<commit_message>
Auto loan code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NewApp_CustomerDetailsTestData" sheetId="1" r:id="rId1"/>
-    <sheet name="NewAppExecution" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Facility_info_TestData" sheetId="3" r:id="rId2"/>
+    <sheet name="NewAppExecution" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -54,12 +55,6 @@
     <t>10-Aug-1998</t>
   </si>
   <si>
-    <t>AT_APP_03</t>
-  </si>
-  <si>
-    <t>DS01_AT_APP_03</t>
-  </si>
-  <si>
     <t>AT_AL_CUSDETAILS_02</t>
   </si>
   <si>
@@ -121,6 +116,294 @@
   </si>
   <si>
     <t>abcd</t>
+  </si>
+  <si>
+    <t>application_type</t>
+  </si>
+  <si>
+    <t>salutation</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>middle_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>father_first_name</t>
+  </si>
+  <si>
+    <t>father_middle_name</t>
+  </si>
+  <si>
+    <t>father_last_name</t>
+  </si>
+  <si>
+    <t>spouse_first_name</t>
+  </si>
+  <si>
+    <t>spouse_middle_name</t>
+  </si>
+  <si>
+    <t>spouse_last_name</t>
+  </si>
+  <si>
+    <t>no_of_children</t>
+  </si>
+  <si>
+    <t>spouse_status</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>education_level</t>
+  </si>
+  <si>
+    <t>maritail_status</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>residential_status</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>no_of_dependents</t>
+  </si>
+  <si>
+    <t>mothers_maiden_name</t>
+  </si>
+  <si>
+    <t>type_of_residency</t>
+  </si>
+  <si>
+    <t>industry_segmentation</t>
+  </si>
+  <si>
+    <t>is_income_considered</t>
+  </si>
+  <si>
+    <t>customer_profile</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>politically_exposed</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>mobile_number_primary</t>
+  </si>
+  <si>
+    <t>mobile_number_secondary</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>prefered_contact_method</t>
+  </si>
+  <si>
+    <t>prefered_time_for_contact</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>test098@gmail.com</t>
+  </si>
+  <si>
+    <t>9654120147</t>
+  </si>
+  <si>
+    <t>9657785656</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>SON</t>
+  </si>
+  <si>
+    <t>Small Software Companies. (Small Software Companies have an employee strength less than 50 people or total turnover less than Rs.50 crore)</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Accomodation</t>
+  </si>
+  <si>
+    <t>Self owned</t>
+  </si>
+  <si>
+    <t>Shushma</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Resident</t>
+  </si>
+  <si>
+    <t>HINDU</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>10-Oct-1998</t>
+  </si>
+  <si>
+    <t>Not Working</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Primary Applicant</t>
+  </si>
+  <si>
+    <t>9874556328</t>
+  </si>
+  <si>
+    <t>customer_type_dropdown</t>
+  </si>
+  <si>
+    <t>search_date_of_birth</t>
+  </si>
+  <si>
+    <t>Clsification</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>scheme</t>
+  </si>
+  <si>
+    <t>program_code</t>
+  </si>
+  <si>
+    <t>facility_type</t>
+  </si>
+  <si>
+    <t>servicing_branch</t>
+  </si>
+  <si>
+    <t>pricing_or_interest_indecator</t>
+  </si>
+  <si>
+    <t>requested_amount</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>loan_tenure</t>
+  </si>
+  <si>
+    <t>Auto Loan</t>
+  </si>
+  <si>
+    <t>Auto Loan-Auto Loan Scheme</t>
+  </si>
+  <si>
+    <t>Auto Loan Standard Scheme</t>
+  </si>
+  <si>
+    <t>Income Based</t>
+  </si>
+  <si>
+    <t>Auto Leasing Loan</t>
+  </si>
+  <si>
+    <t>Standard Scheme for Auto_347</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>declared_downpayment_amount</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>1000000</t>
+  </si>
+  <si>
+    <t>AT_AL_FD_01</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_FD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_FD_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_FD_02</t>
+  </si>
+  <si>
+    <t>AT_AL_FD_03</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_FD_03</t>
+  </si>
+  <si>
+    <t>asset_price</t>
+  </si>
+  <si>
+    <t>1800000</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>1400000</t>
   </si>
 </sst>
 </file>
@@ -156,7 +439,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +491,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,8 +555,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -277,6 +564,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
@@ -573,146 +862,581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="6" customWidth="1"/>
-    <col min="5" max="6" width="29.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="41.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="22.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="29.7109375" style="4" customWidth="1"/>
+    <col min="7" max="45" width="41.42578125" style="4" customWidth="1"/>
+    <col min="46" max="46" width="21.85546875" style="4" customWidth="1"/>
+    <col min="47" max="47" width="23.85546875" style="4" customWidth="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:48">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="W1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AV1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:48">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC2" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD2" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT2" s="13"/>
+      <c r="AU2" s="13"/>
+      <c r="AV2" s="13"/>
+    </row>
+    <row r="3" spans="1:48">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
+      <c r="AR3" s="13"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="AU3" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="AV3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="AQ2" r:id="rId1"/>
+    <hyperlink ref="AU3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32" style="4" customWidth="1"/>
+    <col min="5" max="5" width="29" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20" style="4" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="40.140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" style="4" customWidth="1"/>
+    <col min="13" max="14" width="39.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="23" style="4" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="7">
+        <v>60</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -728,73 +1452,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>26</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="B5" s="4"/>
+      <c r="A5" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Tawruqq dta check code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="241">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -739,6 +739,9 @@
   </si>
   <si>
     <t>4637</t>
+  </si>
+  <si>
+    <t>4672</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1517,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Ijarah living expense code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="242">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -742,6 +742,9 @@
   </si>
   <si>
     <t>4672</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1517,7 +1520,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated code commit 22 01 2024
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="244">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -748,6 +748,9 @@
   </si>
   <si>
     <t>4982</t>
+  </si>
+  <si>
+    <t>4992</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1526,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Income details code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="244">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1526,7 +1526,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Disbursement maker checker code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationDetails_NewApp" sheetId="5" r:id="rId1"/>
@@ -12,14 +12,18 @@
     <sheet name="Facility_info_TestData" sheetId="3" r:id="rId3"/>
     <sheet name="AppDataEntry_EmploymentTestData" sheetId="6" r:id="rId4"/>
     <sheet name="AppDataEntry_FacilityInfoData" sheetId="7" r:id="rId5"/>
-    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId6"/>
+    <sheet name="DBMRBeneficiaryDetails_TestData" sheetId="8" r:id="rId6"/>
+    <sheet name="DMRCR_AplicationDetailsTestData" sheetId="9" r:id="rId7"/>
+    <sheet name="DMRCR_FacilityInfoTestData" sheetId="10" r:id="rId8"/>
+    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId9"/>
+    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="292">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -543,9 +547,6 @@
     <t>DS01_AT_AL_APPDETAILS_03</t>
   </si>
   <si>
-    <t>4272</t>
-  </si>
-  <si>
     <t>AT_AL_APPDATAENTRY_REFDETAILS_01</t>
   </si>
   <si>
@@ -726,38 +727,184 @@
     <t>BT Topup</t>
   </si>
   <si>
-    <t>4494</t>
-  </si>
-  <si>
-    <t>4497</t>
-  </si>
-  <si>
-    <t>4577</t>
-  </si>
-  <si>
-    <t>4611</t>
-  </si>
-  <si>
-    <t>4637</t>
-  </si>
-  <si>
-    <t>4672</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>4982</t>
-  </si>
-  <si>
-    <t>4992</t>
+    <t>facility_application_id</t>
+  </si>
+  <si>
+    <t>beneficiary_name</t>
+  </si>
+  <si>
+    <t>beneficiary_type</t>
+  </si>
+  <si>
+    <t>beneficiary_kyc</t>
+  </si>
+  <si>
+    <t>beneficiary_address</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>iban_account_no</t>
+  </si>
+  <si>
+    <t>micr_type</t>
+  </si>
+  <si>
+    <t>beneficiary_micr_code</t>
+  </si>
+  <si>
+    <t>bank_code</t>
+  </si>
+  <si>
+    <t>branch_name</t>
+  </si>
+  <si>
+    <t>ifsc_code</t>
+  </si>
+  <si>
+    <t>payment_type</t>
+  </si>
+  <si>
+    <t>payment_mode</t>
+  </si>
+  <si>
+    <t>beneficiary_email</t>
+  </si>
+  <si>
+    <t>Auto Loan Scheme</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>car street</t>
+  </si>
+  <si>
+    <t>Savings Account</t>
+  </si>
+  <si>
+    <t>7452136547896</t>
+  </si>
+  <si>
+    <t>MICR</t>
+  </si>
+  <si>
+    <t>SIB0056</t>
+  </si>
+  <si>
+    <t>SIB</t>
+  </si>
+  <si>
+    <t>Dammam Branch</t>
+  </si>
+  <si>
+    <t>SBIN9876</t>
+  </si>
+  <si>
+    <t>On Completion</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>test987@gmail.com</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_01_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_BD_DMC_01_02</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_03</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_BD_DMC_03</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_04</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_BD_DMC_04</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_05</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_06</t>
+  </si>
+  <si>
+    <t>return_stage</t>
+  </si>
+  <si>
+    <t>return_remark</t>
+  </si>
+  <si>
+    <t>Automation return</t>
+  </si>
+  <si>
+    <t>DS01_AT_AD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>loan_amount</t>
+  </si>
+  <si>
+    <t>15,00,000.00</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_01_01</t>
+  </si>
+  <si>
+    <t>DS01_AT_AD_AL_DMC_01_01</t>
+  </si>
+  <si>
+    <t>Disbursment Maker</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_03</t>
+  </si>
+  <si>
+    <t>DS01_AT_AD_AL_DMC_03</t>
+  </si>
+  <si>
+    <t>AT_FD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>Ds01_AT_FD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>reject_remark</t>
+  </si>
+  <si>
+    <t>record_rejected</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_02</t>
+  </si>
+  <si>
+    <t>Ds01_AT_AD_AL_DMC_02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -862,7 +1009,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -900,6 +1047,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -909,7 +1106,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -930,6 +1127,24 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
@@ -1228,45 +1443,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4:W4"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
-    <col min="22" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
-    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -1334,10 +1548,10 @@
         <v>146</v>
       </c>
       <c r="V1" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="X1" s="5" t="s">
         <v>147</v>
@@ -1433,7 +1647,7 @@
         <v>164</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>30</v>
@@ -1448,7 +1662,7 @@
         <v>162</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AB2" s="7" t="s">
         <v>165</v>
@@ -1526,7 +1740,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -1583,7 +1797,7 @@
         <v>164</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>30</v>
@@ -1598,7 +1812,7 @@
         <v>162</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AB4" s="7" t="s">
         <v>165</v>
@@ -1619,6 +1833,147 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" s="29"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1632,16 +1987,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
-    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
-    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -2020,24 +2375,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -2246,28 +2601,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -2278,73 +2633,73 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>198</v>
-      </c>
       <c r="O1" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>203</v>
-      </c>
       <c r="T1" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="W1" s="5" t="s">
-        <v>208</v>
-      </c>
       <c r="X1" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="Z1" s="5" t="s">
         <v>62</v>
@@ -2352,19 +2707,19 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>176</v>
-      </c>
       <c r="C2" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -2390,76 +2745,76 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>187</v>
-      </c>
       <c r="I3" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J3" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>192</v>
-      </c>
       <c r="L3" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="P3" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="R3" s="7" t="s">
+      <c r="S3" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="T3" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="S3" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y3" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="V3" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="Z3" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2472,29 +2827,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -2555,10 +2910,10 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>109</v>
@@ -2599,10 +2954,10 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2627,10 +2982,10 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -2651,10 +3006,10 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -2679,10 +3034,10 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -2712,22 +3067,408 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="U3" r:id="rId2"/>
+    <hyperlink ref="W4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="F5" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2877,10 +3618,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>24</v>
@@ -2888,10 +3629,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>24</v>
@@ -2899,10 +3640,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>24</v>
@@ -2910,10 +3651,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>24</v>
@@ -2921,10 +3662,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>24</v>
@@ -2932,10 +3673,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>24</v>
@@ -2943,12 +3684,114 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C25" s="29"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" s="35" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Disbursement maker code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="294">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -899,12 +899,19 @@
   </si>
   <si>
     <t>Ds01_AT_AD_AL_DMC_02</t>
+  </si>
+  <si>
+    <t>5233</t>
+  </si>
+  <si>
+    <t>5235</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1449,38 +1456,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
+    <col min="21" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -1740,7 +1747,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>234</v>
+        <v>293</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -1846,13 +1853,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1987,16 +1994,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
+    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -2375,24 +2382,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -2601,28 +2608,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -2833,23 +2840,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -3075,28 +3082,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3319,11 +3326,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3419,9 +3426,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3461,14 +3468,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>

<commit_message>
Disbursement stage code commited
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AnandhULS/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationDetails_NewApp" sheetId="5" r:id="rId1"/>
@@ -15,15 +15,20 @@
     <sheet name="DBMRBeneficiaryDetails_TestData" sheetId="8" r:id="rId6"/>
     <sheet name="DMRCR_AplicationDetailsTestData" sheetId="9" r:id="rId7"/>
     <sheet name="DMRCR_FacilityInfoTestData" sheetId="10" r:id="rId8"/>
-    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId9"/>
-    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId10"/>
+    <sheet name="DMRCR_MarginMoneyTestData" sheetId="12" r:id="rId9"/>
+    <sheet name="DSBMKRCHR_CustmrDetailsTestData" sheetId="13" r:id="rId10"/>
+    <sheet name="DSBMKRCHR_DocDetailsTestData" sheetId="14" r:id="rId11"/>
+    <sheet name="DSBMKRCHR_OfferingTestData" sheetId="15" r:id="rId12"/>
+    <sheet name="DSBMKRCHR_PaymentSchedTestData" sheetId="16" r:id="rId13"/>
+    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId14"/>
+    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="343">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -727,191 +732,337 @@
     <t>BT Topup</t>
   </si>
   <si>
+    <t>facility_application_id</t>
+  </si>
+  <si>
+    <t>beneficiary_name</t>
+  </si>
+  <si>
+    <t>beneficiary_type</t>
+  </si>
+  <si>
+    <t>beneficiary_kyc</t>
+  </si>
+  <si>
+    <t>beneficiary_address</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>iban_account_no</t>
+  </si>
+  <si>
+    <t>micr_type</t>
+  </si>
+  <si>
+    <t>beneficiary_micr_code</t>
+  </si>
+  <si>
+    <t>bank_code</t>
+  </si>
+  <si>
+    <t>branch_name</t>
+  </si>
+  <si>
+    <t>ifsc_code</t>
+  </si>
+  <si>
+    <t>payment_type</t>
+  </si>
+  <si>
+    <t>payment_mode</t>
+  </si>
+  <si>
+    <t>beneficiary_email</t>
+  </si>
+  <si>
+    <t>Auto Loan Scheme</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>car street</t>
+  </si>
+  <si>
+    <t>Savings Account</t>
+  </si>
+  <si>
+    <t>7452136547896</t>
+  </si>
+  <si>
+    <t>MICR</t>
+  </si>
+  <si>
+    <t>SIB0056</t>
+  </si>
+  <si>
+    <t>SIB</t>
+  </si>
+  <si>
+    <t>Dammam Branch</t>
+  </si>
+  <si>
+    <t>SBIN9876</t>
+  </si>
+  <si>
+    <t>On Completion</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>test987@gmail.com</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_01_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_BD_DMC_01_02</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_03</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_BD_DMC_03</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_04</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_BD_DMC_04</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_05</t>
+  </si>
+  <si>
+    <t>AT_AL_BD_DMC_06</t>
+  </si>
+  <si>
+    <t>return_stage</t>
+  </si>
+  <si>
+    <t>return_remark</t>
+  </si>
+  <si>
+    <t>Automation return</t>
+  </si>
+  <si>
+    <t>DS01_AT_AD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>loan_amount</t>
+  </si>
+  <si>
+    <t>15,00,000.00</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_01_01</t>
+  </si>
+  <si>
+    <t>DS01_AT_AD_AL_DMC_01_01</t>
+  </si>
+  <si>
+    <t>Disbursment Maker</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_03</t>
+  </si>
+  <si>
+    <t>DS01_AT_AD_AL_DMC_03</t>
+  </si>
+  <si>
+    <t>AT_FD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>Ds01_AT_FD_AL_DMC_01</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>reject_remark</t>
+  </si>
+  <si>
+    <t>record_rejected</t>
+  </si>
+  <si>
+    <t>AT_AD_AL_DMC_02</t>
+  </si>
+  <si>
+    <t>Ds01_AT_AD_AL_DMC_02</t>
+  </si>
+  <si>
+    <t>own_contribution_amount</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>own_contribution_amount_paid</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_MM_01</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_MM_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_DSB_MM_02</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_MM_03</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_DSB_MM_03</t>
+  </si>
+  <si>
+    <t>Customer_First_Name</t>
+  </si>
+  <si>
+    <t>Customer_last_name</t>
+  </si>
+  <si>
+    <t>AutoProduct</t>
+  </si>
+  <si>
+    <t>AT_ADC_AL_DMC_01_MKR</t>
+  </si>
+  <si>
+    <t>DS01_AT_ADC_AL_DMC_01_MKR</t>
+  </si>
+  <si>
+    <t>AT_ADC_AL_DMC_01_CHR</t>
+  </si>
+  <si>
+    <t>DS01_AT_ADC_AL_DMC_01_CHR</t>
+  </si>
+  <si>
+    <t>AT_AL_DC_01_MKR</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_DC_01_MKR</t>
+  </si>
+  <si>
+    <t>document_name</t>
+  </si>
+  <si>
+    <t>document_status</t>
+  </si>
+  <si>
+    <t>AADHAAR</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>AT_AL_DC_01_CHR</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_DC_01_CHR</t>
+  </si>
+  <si>
+    <t>clasification</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>scheme_ID</t>
+  </si>
+  <si>
+    <t>AT_OFD_AL_DMC_01_MKR</t>
+  </si>
+  <si>
+    <t>DS01_AT_OFD_AL_DMC_01_MKR</t>
+  </si>
+  <si>
+    <t>AT_OFD_AL_DMC_01_CHR</t>
+  </si>
+  <si>
+    <t>DS01_AT_OFD_AL_DMC_01_CHR</t>
+  </si>
+  <si>
+    <t>AT_AL_PS_DSP_01</t>
+  </si>
+  <si>
+    <t>Payment_type</t>
+  </si>
+  <si>
+    <t>payee</t>
+  </si>
+  <si>
+    <t>planned_scheduled_amount</t>
+  </si>
+  <si>
+    <t>schedule_notes</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>AT_AL_PS_DSP_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_PS_DSP_02</t>
+  </si>
+  <si>
+    <t>AT_AL_PS_DSP_03</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_02</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_03</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_04</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_05</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>facility_application_id</t>
-  </si>
-  <si>
-    <t>beneficiary_name</t>
-  </si>
-  <si>
-    <t>beneficiary_type</t>
-  </si>
-  <si>
-    <t>beneficiary_kyc</t>
-  </si>
-  <si>
-    <t>beneficiary_address</t>
-  </si>
-  <si>
-    <t>account_type</t>
-  </si>
-  <si>
-    <t>iban_account_no</t>
-  </si>
-  <si>
-    <t>micr_type</t>
-  </si>
-  <si>
-    <t>beneficiary_micr_code</t>
-  </si>
-  <si>
-    <t>bank_code</t>
-  </si>
-  <si>
-    <t>branch_name</t>
-  </si>
-  <si>
-    <t>ifsc_code</t>
-  </si>
-  <si>
-    <t>payment_type</t>
-  </si>
-  <si>
-    <t>payment_mode</t>
-  </si>
-  <si>
-    <t>beneficiary_email</t>
-  </si>
-  <si>
-    <t>Auto Loan Scheme</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Builder</t>
-  </si>
-  <si>
-    <t>car street</t>
-  </si>
-  <si>
-    <t>Savings Account</t>
-  </si>
-  <si>
-    <t>7452136547896</t>
-  </si>
-  <si>
-    <t>MICR</t>
-  </si>
-  <si>
-    <t>SIB0056</t>
-  </si>
-  <si>
-    <t>SIB</t>
-  </si>
-  <si>
-    <t>Dammam Branch</t>
-  </si>
-  <si>
-    <t>SBIN9876</t>
-  </si>
-  <si>
-    <t>On Completion</t>
-  </si>
-  <si>
-    <t>Cheque</t>
-  </si>
-  <si>
-    <t>test987@gmail.com</t>
-  </si>
-  <si>
-    <t>AT_AL_BD_DMC_01_02</t>
-  </si>
-  <si>
-    <t>DS01_AT_AL_BD_DMC_01_02</t>
-  </si>
-  <si>
-    <t>AT_AL_BD_DMC_03</t>
-  </si>
-  <si>
-    <t>DS01_AT_AL_BD_DMC_03</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>AT_AL_BD_DMC_04</t>
-  </si>
-  <si>
-    <t>DS01_AT_AL_BD_DMC_04</t>
-  </si>
-  <si>
-    <t>AT_AD_AL_DMC_01</t>
-  </si>
-  <si>
-    <t>AT_AL_BD_DMC_05</t>
-  </si>
-  <si>
-    <t>AT_AL_BD_DMC_06</t>
-  </si>
-  <si>
-    <t>return_stage</t>
-  </si>
-  <si>
-    <t>return_remark</t>
-  </si>
-  <si>
-    <t>Automation return</t>
-  </si>
-  <si>
-    <t>DS01_AT_AD_AL_DMC_01</t>
-  </si>
-  <si>
-    <t>loan_amount</t>
-  </si>
-  <si>
-    <t>15,00,000.00</t>
-  </si>
-  <si>
-    <t>AT_AD_AL_DMC_01_01</t>
-  </si>
-  <si>
-    <t>DS01_AT_AD_AL_DMC_01_01</t>
-  </si>
-  <si>
-    <t>Disbursment Maker</t>
-  </si>
-  <si>
-    <t>AT_AD_AL_DMC_03</t>
-  </si>
-  <si>
-    <t>DS01_AT_AD_AL_DMC_03</t>
-  </si>
-  <si>
-    <t>AT_FD_AL_DMC_01</t>
-  </si>
-  <si>
-    <t>Ds01_AT_FD_AL_DMC_01</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>reject_remark</t>
-  </si>
-  <si>
-    <t>record_rejected</t>
-  </si>
-  <si>
-    <t>AT_AD_AL_DMC_02</t>
-  </si>
-  <si>
-    <t>Ds01_AT_AD_AL_DMC_02</t>
-  </si>
-  <si>
-    <t>5233</t>
-  </si>
-  <si>
-    <t>5235</t>
+    <t>AT_AL_DSB_DD_02</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_03</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1113,7 +1264,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -1152,13 +1303,135 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -1451,43 +1724,43 @@
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
-    <col min="21" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
-    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -1747,7 +2020,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>293</v>
+        <v>339</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -1845,21 +2118,310 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="22" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1889,11 +2451,591 @@
       </c>
     </row>
     <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="C29" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B46" s="18"/>
+      <c r="C46" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="B47" s="18"/>
+      <c r="C47" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="C48" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="B49" s="18"/>
+      <c r="C49" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="B50" s="18"/>
+      <c r="C50" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C49">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>264</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>265</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>24</v>
@@ -1901,10 +3043,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>266</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>267</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>24</v>
@@ -1912,10 +3054,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>270</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>24</v>
@@ -1923,17 +3065,17 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>24</v>
@@ -1941,16 +3083,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34" t="s">
@@ -1959,10 +3101,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>285</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>286</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>24</v>
@@ -1970,10 +3112,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>283</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>284</v>
       </c>
       <c r="C10" s="35" t="s">
         <v>24</v>
@@ -1989,21 +3131,21 @@
   <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
-    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
-    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -2377,29 +3519,29 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:R5"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -2603,33 +3745,33 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -2835,28 +3977,28 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -3077,33 +4219,33 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3114,49 +4256,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>248</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>249</v>
       </c>
       <c r="R1" s="18" t="s">
         <v>62</v>
@@ -3179,55 +4321,55 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>265</v>
-      </c>
       <c r="C2" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="I2" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="M2" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="N2" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="O2" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="P2" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="Q2" s="21" t="s">
         <v>262</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>263</v>
       </c>
       <c r="R2" s="20" t="s">
         <v>211</v>
@@ -3240,10 +4382,10 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>266</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>267</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -3265,7 +4407,7 @@
         <v>32</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U3" s="8" t="s">
         <v>31</v>
@@ -3275,10 +4417,10 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>270</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -3300,7 +4442,7 @@
       <c r="T4" s="23"/>
       <c r="U4" s="23"/>
       <c r="V4" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="W4" s="8" t="s">
         <v>31</v>
@@ -3320,17 +4462,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3341,27 +4483,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>275</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -3369,13 +4511,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>281</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
@@ -3383,31 +4525,31 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="25" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>290</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>291</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>283</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>284</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F5" s="26"/>
     </row>
@@ -3421,14 +4563,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3444,13 +4586,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="31" t="s">
         <v>286</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -3460,349 +4602,87 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>295</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="22" t="s">
-        <v>269</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="29"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="C25" s="29"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>24</v>
+        <v>299</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>